<commit_message>
Added another tab with unique codes per missing language
</commit_message>
<xml_diff>
--- a/terminology/snomed-missing-translations.xlsx
+++ b/terminology/snomed-missing-translations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\HdBe-FHIR-R4-CBB\terminology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\hdbe-fhir-r4-cbb\terminology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEC1A29-55CC-4922-8302-93E0BB312761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE8B01D4-3AFA-485B-8BA6-34AC1AD4966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48A0F11F-E4C3-4C20-A482-6DCAE6188D16}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48A0F11F-E4C3-4C20-A482-6DCAE6188D16}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Deduplicated" sheetId="2" r:id="rId1"/>
+    <sheet name="All codes" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="106">
   <si>
     <t>ValueSet-AlcoholUseStatus.xml</t>
   </si>
@@ -338,6 +339,21 @@
   </si>
   <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Missing language</t>
+  </si>
+  <si>
+    <t>SNOMED Code</t>
   </si>
 </sst>
 </file>
@@ -694,16 +710,1051 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BF5269-0CD6-4FA0-A695-13D950B9881F}">
-  <dimension ref="A1:D179"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A199E-C749-464F-90C8-ABEF40DFF849}">
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10179008</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10179008</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>14803004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>14803004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>22762002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>22762002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>26643006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>26643006</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>33553000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>33553000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>46713006</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>46713006</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>47625008</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>47625008</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>69620002</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>69620002</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>74964007</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>74964007</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>84638005</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>84638005</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>89925002</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>89925002</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>125681006</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>125681006</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>160504008</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>160708008</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>183446009</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>183446009</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>183966005</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>184003006</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>186065003</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>186065003</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>224152001</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>224670004</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>224670004</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>248160001</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>255545003</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>255545003</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>257564005</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>257564005</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>257630004</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>257630004</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>257641002</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>257641002</v>
+      </c>
+      <c r="B45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>260413007</v>
+      </c>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>260413007</v>
+      </c>
+      <c r="B47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>261665006</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>261665006</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>263718001</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>263718001</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>274512008</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>276727009</v>
+      </c>
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>276727009</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>277132007</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>371911009</v>
+      </c>
+      <c r="B56" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>385643006</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>385643006</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>385655000</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>385655000</v>
+      </c>
+      <c r="B60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>405613005</v>
+      </c>
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>406149000</v>
+      </c>
+      <c r="B62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>408366001</v>
+      </c>
+      <c r="B63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>410521004</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>410521004</v>
+      </c>
+      <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>417284009</v>
+      </c>
+      <c r="B66" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>417284009</v>
+      </c>
+      <c r="B67" t="s">
+        <v>39</v>
+      </c>
+      <c r="C67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>423155007</v>
+      </c>
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>423527000</v>
+      </c>
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>424415008</v>
+      </c>
+      <c r="B70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>424661000</v>
+      </c>
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>424948003</v>
+      </c>
+      <c r="B72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>447694001</v>
+      </c>
+      <c r="B73" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>447694001</v>
+      </c>
+      <c r="B74" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>465153004</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>465153004</v>
+      </c>
+      <c r="B76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>704417003</v>
+      </c>
+      <c r="B77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>705046008</v>
+      </c>
+      <c r="B78" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>705390009</v>
+      </c>
+      <c r="B79" t="s">
+        <v>46</v>
+      </c>
+      <c r="C79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>705390009</v>
+      </c>
+      <c r="B80" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>705401004</v>
+      </c>
+      <c r="B81" t="s">
+        <v>45</v>
+      </c>
+      <c r="C81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>705401004</v>
+      </c>
+      <c r="B82" t="s">
+        <v>45</v>
+      </c>
+      <c r="C82" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>713914004</v>
+      </c>
+      <c r="B83" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>715758005</v>
+      </c>
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>715881003</v>
+      </c>
+      <c r="B85" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>722499006</v>
+      </c>
+      <c r="B86" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>768832004</v>
+      </c>
+      <c r="B87" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>768832004</v>
+      </c>
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>783261004</v>
+      </c>
+      <c r="B89" t="s">
+        <v>70</v>
+      </c>
+      <c r="C89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>785889008</v>
+      </c>
+      <c r="B90" t="s">
+        <v>97</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>786063001</v>
+      </c>
+      <c r="B91" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>3.25706810000361E+16</v>
+      </c>
+      <c r="B92" t="s">
+        <v>74</v>
+      </c>
+      <c r="C92" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F104">
+    <sortCondition ref="A2:A104"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BF5269-0CD6-4FA0-A695-13D950B9881F}">
+  <dimension ref="A1:D179"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:B179"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.21875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>